<commit_message>
create script to generate results
</commit_message>
<xml_diff>
--- a/Scripts/inclusion_stats.xlsx
+++ b/Scripts/inclusion_stats.xlsx
@@ -14,15 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="10">
   <si>
-    <t>../Data/Data_0_Synergy.csv</t>
+    <t>Data_0_Synergy.csv</t>
   </si>
   <si>
-    <t>../Data/Data_1_old_replication.csv</t>
+    <t>Data_1_old_replication.csv</t>
   </si>
   <si>
-    <t>../Data/Data_2_old_comprehensive.csv</t>
+    <t>Data_2_old_comprehensive.csv</t>
   </si>
   <si>
     <t>Data_4a_snowballing.csv</t>
@@ -401,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -557,7 +557,7 @@
         <v>9</v>
       </c>
       <c r="G6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H6">
         <v>9</v>
@@ -583,7 +583,7 @@
         <v>9</v>
       </c>
       <c r="G7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H7">
         <v>9</v>
@@ -669,7 +669,7 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
@@ -678,7 +678,7 @@
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E11" t="s">
         <v>8</v>
@@ -707,13 +707,13 @@
         <v>9</v>
       </c>
       <c r="E12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H12">
         <v>5</v>
@@ -750,25 +750,25 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E14" t="s">
         <v>9</v>
       </c>
       <c r="F14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G14" t="s">
         <v>9</v>
       </c>
       <c r="H14">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -776,10 +776,10 @@
         <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D15" t="s">
         <v>8</v>
@@ -791,10 +791,10 @@
         <v>8</v>
       </c>
       <c r="G15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H15">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -831,22 +831,22 @@
         <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D17" t="s">
         <v>8</v>
       </c>
       <c r="E17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F17" t="s">
         <v>8</v>
       </c>
       <c r="G17" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H17">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -880,13 +880,13 @@
         <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C19" t="s">
         <v>8</v>
       </c>
       <c r="D19" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E19" t="s">
         <v>8</v>
@@ -895,7 +895,7 @@
         <v>8</v>
       </c>
       <c r="G19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H19">
         <v>2</v>
@@ -912,16 +912,16 @@
         <v>8</v>
       </c>
       <c r="D20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E20" t="s">
         <v>8</v>
       </c>
       <c r="F20" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G20" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H20">
         <v>2</v>
@@ -932,7 +932,7 @@
         <v>8</v>
       </c>
       <c r="B21" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C21" t="s">
         <v>8</v>
@@ -941,16 +941,16 @@
         <v>8</v>
       </c>
       <c r="E21" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G21" t="s">
         <v>9</v>
       </c>
       <c r="H21">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -961,7 +961,7 @@
         <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D22" t="s">
         <v>8</v>
@@ -970,10 +970,10 @@
         <v>9</v>
       </c>
       <c r="F22" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H22">
         <v>1</v>
@@ -984,7 +984,7 @@
         <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C23" t="s">
         <v>9</v>
@@ -993,10 +993,10 @@
         <v>8</v>
       </c>
       <c r="E23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G23" t="s">
         <v>8</v>
@@ -1013,19 +1013,19 @@
         <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D24" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E24" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F24" t="s">
         <v>8</v>
       </c>
       <c r="G24" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H24">
         <v>1</v>
@@ -1045,10 +1045,10 @@
         <v>9</v>
       </c>
       <c r="E25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F25" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G25" t="s">
         <v>9</v>
@@ -1068,10 +1068,10 @@
         <v>8</v>
       </c>
       <c r="D26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E26" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F26" t="s">
         <v>9</v>
@@ -1085,10 +1085,10 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C27" t="s">
         <v>8</v>
@@ -1100,7 +1100,7 @@
         <v>8</v>
       </c>
       <c r="F27" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G27" t="s">
         <v>8</v>
@@ -1117,73 +1117,21 @@
         <v>8</v>
       </c>
       <c r="C28" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D28" t="s">
         <v>8</v>
       </c>
       <c r="E28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G28" t="s">
         <v>9</v>
       </c>
       <c r="H28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
-      <c r="A29" t="s">
-        <v>8</v>
-      </c>
-      <c r="B29" t="s">
-        <v>8</v>
-      </c>
-      <c r="C29" t="s">
-        <v>8</v>
-      </c>
-      <c r="D29" t="s">
-        <v>8</v>
-      </c>
-      <c r="E29" t="s">
-        <v>8</v>
-      </c>
-      <c r="F29" t="s">
-        <v>9</v>
-      </c>
-      <c r="G29" t="s">
-        <v>8</v>
-      </c>
-      <c r="H29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="A30" t="s">
-        <v>8</v>
-      </c>
-      <c r="B30" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" t="s">
-        <v>9</v>
-      </c>
-      <c r="D30" t="s">
-        <v>8</v>
-      </c>
-      <c r="E30" t="s">
-        <v>8</v>
-      </c>
-      <c r="F30" t="s">
-        <v>8</v>
-      </c>
-      <c r="G30" t="s">
-        <v>9</v>
-      </c>
-      <c r="H30">
         <v>1</v>
       </c>
     </row>

</xml_diff>